<commit_message>
Projektabschnitt 5: - Eingabe und Auslese sowie Prüfen - aktualisieren der Datenbank mit Eingegebenen Daten
</commit_message>
<xml_diff>
--- a/Documents/Dokumentation/Projektphasen.xlsx
+++ b/Documents/Dokumentation/Projektphasen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AD5414-5773-49FC-A4D8-C1090FF27518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D29A711-C947-4292-92EB-84858A127418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11835" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3316,7 +3316,7 @@
   <dimension ref="A2:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3738,11 +3738,11 @@
         <v>4</v>
       </c>
       <c r="C34">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="D34">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>1.75</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,11 +3929,11 @@
       </c>
       <c r="C50">
         <f>SUBTOTAL(109,Tabelle245687[Ist])</f>
-        <v>77.25</v>
+        <v>77.75</v>
       </c>
       <c r="D50">
         <f>SUBTOTAL(109,Tabelle245687[Differenz])</f>
-        <v>146.75</v>
+        <v>146.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projektabschnitt 5: - Prüfen ob unbearbeitete Aufgaben vorhanden sind - unbearbeitete Aufgaben anzeigen
</commit_message>
<xml_diff>
--- a/Documents/Dokumentation/Projektphasen.xlsx
+++ b/Documents/Dokumentation/Projektphasen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D29A711-C947-4292-92EB-84858A127418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A82933B-9A2F-4C9E-909E-615323FDA960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11835" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3738,11 +3738,11 @@
         <v>4</v>
       </c>
       <c r="C34">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="D34">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,11 +3929,11 @@
       </c>
       <c r="C50">
         <f>SUBTOTAL(109,Tabelle245687[Ist])</f>
-        <v>77.75</v>
+        <v>78.25</v>
       </c>
       <c r="D50">
         <f>SUBTOTAL(109,Tabelle245687[Differenz])</f>
-        <v>146.25</v>
+        <v>145.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projektabschnitt 5: - Aufgabenblätter in home.html anzeigen
</commit_message>
<xml_diff>
--- a/Documents/Dokumentation/Projektphasen.xlsx
+++ b/Documents/Dokumentation/Projektphasen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9C524C-30CF-4A6C-966D-04A79C510577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80E06D9-C1F0-4869-9B90-1E5B3D473C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11835" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3316,7 +3316,7 @@
   <dimension ref="A2:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3708,11 +3708,11 @@
         <v>8</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>4.75</v>
       </c>
       <c r="D32">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>4</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,11 +3929,11 @@
       </c>
       <c r="C50">
         <f>SUBTOTAL(109,Tabelle245687[Ist])</f>
-        <v>78.75</v>
+        <v>79.5</v>
       </c>
       <c r="D50">
         <f>SUBTOTAL(109,Tabelle245687[Differenz])</f>
-        <v>145.25</v>
+        <v>144.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projektabschnitt 5: - Aufgabenblätter in home.html anzeigen - ermöglichen Aufruf Aufgabenblätter - unvollständig!!
</commit_message>
<xml_diff>
--- a/Documents/Dokumentation/Projektphasen.xlsx
+++ b/Documents/Dokumentation/Projektphasen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80E06D9-C1F0-4869-9B90-1E5B3D473C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7EEDDD-1674-47CB-9C62-81100764AFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11835" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3708,11 +3708,11 @@
         <v>8</v>
       </c>
       <c r="C32">
-        <v>4.75</v>
+        <v>5.5</v>
       </c>
       <c r="D32">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,11 +3929,11 @@
       </c>
       <c r="C50">
         <f>SUBTOTAL(109,Tabelle245687[Ist])</f>
-        <v>79.5</v>
+        <v>80.25</v>
       </c>
       <c r="D50">
         <f>SUBTOTAL(109,Tabelle245687[Differenz])</f>
-        <v>144.5</v>
+        <v>143.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projektabschnitt 5: - Aufgabenblätter in home.html anzeigen - home überarbeitet
</commit_message>
<xml_diff>
--- a/Documents/Dokumentation/Projektphasen.xlsx
+++ b/Documents/Dokumentation/Projektphasen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F0A616-C03F-423B-9BEE-3B46C157F52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE29F6C-A28F-4BAD-9DFA-BA24B6C45325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11835" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3316,7 +3316,7 @@
   <dimension ref="A2:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3708,11 +3708,11 @@
         <v>8</v>
       </c>
       <c r="C32">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="D32">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,11 +3929,11 @@
       </c>
       <c r="C50">
         <f>SUBTOTAL(109,Tabelle245687[Ist])</f>
-        <v>81.25</v>
+        <v>81.75</v>
       </c>
       <c r="D50">
         <f>SUBTOTAL(109,Tabelle245687[Differenz])</f>
-        <v>142.75</v>
+        <v>142.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projektabschnitt 5: - Themengebiete aussuchen - home.html überarbeitet - unvollständig!
</commit_message>
<xml_diff>
--- a/Documents/Dokumentation/Projektphasen.xlsx
+++ b/Documents/Dokumentation/Projektphasen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE29F6C-A28F-4BAD-9DFA-BA24B6C45325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26C7475-7876-4B5D-8816-4B6BD75A018B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11835" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3316,7 +3316,7 @@
   <dimension ref="A2:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3708,11 +3708,11 @@
         <v>8</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>6.75</v>
       </c>
       <c r="D32">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,11 +3929,11 @@
       </c>
       <c r="C50">
         <f>SUBTOTAL(109,Tabelle245687[Ist])</f>
-        <v>81.75</v>
+        <v>82.5</v>
       </c>
       <c r="D50">
         <f>SUBTOTAL(109,Tabelle245687[Differenz])</f>
-        <v>142.25</v>
+        <v>141.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projektabschnitt 5: - Themengebiete aussuchen
</commit_message>
<xml_diff>
--- a/Documents/Dokumentation/Projektphasen.xlsx
+++ b/Documents/Dokumentation/Projektphasen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26C7475-7876-4B5D-8816-4B6BD75A018B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648F3BD2-06B3-4F5E-A3C0-4AB85917DE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11835" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3316,7 +3316,7 @@
   <dimension ref="A2:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3708,11 +3708,11 @@
         <v>8</v>
       </c>
       <c r="C32">
-        <v>6.75</v>
+        <v>7</v>
       </c>
       <c r="D32">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3738,11 +3738,11 @@
         <v>4</v>
       </c>
       <c r="C34">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="D34">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3912,11 +3912,11 @@
         <v>10</v>
       </c>
       <c r="C49">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="D49">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>6</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,11 +3929,11 @@
       </c>
       <c r="C50">
         <f>SUBTOTAL(109,Tabelle245687[Ist])</f>
-        <v>82.5</v>
+        <v>83.25</v>
       </c>
       <c r="D50">
         <f>SUBTOTAL(109,Tabelle245687[Differenz])</f>
-        <v>141.5</v>
+        <v>140.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projektabschnitt 5: - Abschluss Projektabschnitt 5 - Grundfunktionen erfüllt
</commit_message>
<xml_diff>
--- a/Documents/Dokumentation/Projektphasen.xlsx
+++ b/Documents/Dokumentation/Projektphasen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A4A2A4-FC36-4CD9-917E-42C7DDF7DE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4812234-31E3-452B-B901-57DCB3167638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="4020" windowWidth="21600" windowHeight="11835" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3315,8 +3315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E002C3-AD10-485D-929B-ACE9922C7AED}">
   <dimension ref="A2:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3723,11 +3723,11 @@
         <v>4</v>
       </c>
       <c r="C33">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>3.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,11 +3929,11 @@
       </c>
       <c r="C50">
         <f>SUBTOTAL(109,Tabelle245687[Ist])</f>
-        <v>83.25</v>
+        <v>83.75</v>
       </c>
       <c r="D50">
         <f>SUBTOTAL(109,Tabelle245687[Differenz])</f>
-        <v>140.75</v>
+        <v>140.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dokumentation: - Projektabschnitt 5 - Verzeichnisse aktualisieren - Abbildungen, etc.
</commit_message>
<xml_diff>
--- a/Documents/Dokumentation/Projektphasen.xlsx
+++ b/Documents/Dokumentation/Projektphasen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4812234-31E3-452B-B901-57DCB3167638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A630567-F3B8-45B9-A7BD-54E734E8557F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="4020" windowWidth="21600" windowHeight="11835" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4365" yWindow="4365" windowWidth="21600" windowHeight="11835" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorl. Antrag" sheetId="1" r:id="rId1"/>
@@ -3315,8 +3315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E002C3-AD10-485D-929B-ACE9922C7AED}">
   <dimension ref="A2:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3856,11 +3856,11 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>6</v>
+        <v>6.75</v>
       </c>
       <c r="D44">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>3</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,11 +3929,11 @@
       </c>
       <c r="C50">
         <f>SUBTOTAL(109,Tabelle245687[Ist])</f>
-        <v>83.75</v>
+        <v>84.5</v>
       </c>
       <c r="D50">
         <f>SUBTOTAL(109,Tabelle245687[Differenz])</f>
-        <v>140.25</v>
+        <v>139.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Abschlusstest Projektabschnitt 1 - 5 - erfolgreich - korrigieren kleiner Probleme   - Subjects wurde nicht erstellt, behoben   - chooseExercises <= 1 geändert
</commit_message>
<xml_diff>
--- a/Documents/Dokumentation/Projektphasen.xlsx
+++ b/Documents/Dokumentation/Projektphasen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C08A83-0825-4CA0-B62C-CA7C0C14A0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889EFF56-8484-4429-B79D-E8E278D33ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4365" yWindow="4365" windowWidth="21600" windowHeight="11835" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3316,7 +3316,7 @@
   <dimension ref="A2:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3806,11 +3806,11 @@
         <v>20</v>
       </c>
       <c r="C40">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D40">
         <f>Tabelle245687[[#This Row],[Geplant]]-Tabelle245687[[#This Row],[Ist]]</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,11 +3929,11 @@
       </c>
       <c r="C50">
         <f>SUBTOTAL(109,Tabelle245687[Ist])</f>
-        <v>85.75</v>
+        <v>86.75</v>
       </c>
       <c r="D50">
         <f>SUBTOTAL(109,Tabelle245687[Differenz])</f>
-        <v>138.25</v>
+        <v>137.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>